<commit_message>
Add Test Engineer and Delivery Manager descriptors + update skill levels sheet
</commit_message>
<xml_diff>
--- a/GDD_Skill_Levels_descriptions.xlsx
+++ b/GDD_Skill_Levels_descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve.newman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard.raybould/GDD-Evidence-Evaluator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E2679D8-143D-5942-BD5E-014D341630E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3594B3-880B-3D41-AF17-B183C52140F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18120" xr2:uid="{E3A2C896-5453-DA42-8F79-D0CA852F103D}"/>
+    <workbookView xWindow="4020" yWindow="1000" windowWidth="21360" windowHeight="17640" xr2:uid="{E3A2C896-5453-DA42-8F79-D0CA852F103D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="62">
   <si>
     <t>Capability</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>Senior developer - management</t>
+  </si>
+  <si>
+    <t>Senior developer</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Junior Developer</t>
   </si>
 </sst>
 </file>
@@ -644,15 +653,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7AC9B1-ABB7-BD42-B8A5-87DDE96F229D}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124:D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -669,7 +679,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -683,7 +693,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -697,7 +707,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="372" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -711,7 +721,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -725,7 +735,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="404" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -739,7 +749,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -753,7 +763,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -767,7 +777,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -781,7 +791,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -795,7 +805,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -809,7 +819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -823,7 +833,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="356" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -837,7 +847,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -851,7 +861,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="323" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -865,7 +875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -879,7 +889,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -893,7 +903,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -907,7 +917,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -921,7 +931,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="404" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -935,7 +945,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -949,7 +959,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -963,7 +973,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -977,7 +987,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="356" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -991,7 +1001,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1005,7 +1015,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1019,7 +1029,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1033,7 +1043,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1047,7 +1057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1061,7 +1071,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1075,7 +1085,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1089,7 +1099,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1103,7 +1113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1131,7 +1141,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1145,7 +1155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -1159,7 +1169,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1187,7 +1197,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="356" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1201,7 +1211,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1215,7 +1225,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1227,6 +1237,1686 @@
       </c>
       <c r="D41" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D72" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>47</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D75" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>47</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D77" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D78" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D80" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D91" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D92" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D94" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>26</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D95" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D97" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>27</v>
+      </c>
+      <c r="B98" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B99" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>27</v>
+      </c>
+      <c r="B100" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D100" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>27</v>
+      </c>
+      <c r="B101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D101" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>32</v>
+      </c>
+      <c r="B102" t="s">
+        <v>4</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>32</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D103" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>32</v>
+      </c>
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D104" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D105" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>37</v>
+      </c>
+      <c r="B106" t="s">
+        <v>4</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D106" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>37</v>
+      </c>
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D107" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>37</v>
+      </c>
+      <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D108" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>37</v>
+      </c>
+      <c r="B109" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D109" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>42</v>
+      </c>
+      <c r="B110" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D110" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>42</v>
+      </c>
+      <c r="B111" t="s">
+        <v>6</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D111" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>42</v>
+      </c>
+      <c r="B112" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D112" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>42</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D113" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>47</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D114" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>47</v>
+      </c>
+      <c r="B115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D115" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>47</v>
+      </c>
+      <c r="B116" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D116" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>47</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D117" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>52</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D118" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>52</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D119" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>52</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D120" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>52</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D121" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D123" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>3</v>
+      </c>
+      <c r="B125" t="s">
+        <v>8</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D125" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>3</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" t="s">
+        <v>4</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>12</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" t="s">
+        <v>8</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D130" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" t="s">
+        <v>4</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D131" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D132" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>17</v>
+      </c>
+      <c r="B133" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D133" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>17</v>
+      </c>
+      <c r="B134" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D134" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>26</v>
+      </c>
+      <c r="B135" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D135" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>26</v>
+      </c>
+      <c r="B136" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D136" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>26</v>
+      </c>
+      <c r="B137" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>26</v>
+      </c>
+      <c r="B138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D138" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>27</v>
+      </c>
+      <c r="B139" t="s">
+        <v>4</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D139" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>27</v>
+      </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D140" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B141" t="s">
+        <v>8</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D141" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>27</v>
+      </c>
+      <c r="B142" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D142" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>32</v>
+      </c>
+      <c r="B143" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D143" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>32</v>
+      </c>
+      <c r="B144" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D144" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>32</v>
+      </c>
+      <c r="B145" t="s">
+        <v>8</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D145" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>32</v>
+      </c>
+      <c r="B146" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D146" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>37</v>
+      </c>
+      <c r="B147" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D147" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>37</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D148" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>37</v>
+      </c>
+      <c r="B149" t="s">
+        <v>8</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D149" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>37</v>
+      </c>
+      <c r="B150" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D150" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>42</v>
+      </c>
+      <c r="B151" t="s">
+        <v>4</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D151" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>42</v>
+      </c>
+      <c r="B152" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D152" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>42</v>
+      </c>
+      <c r="B153" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D153" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>42</v>
+      </c>
+      <c r="B154" t="s">
+        <v>9</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D154" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>47</v>
+      </c>
+      <c r="B155" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>47</v>
+      </c>
+      <c r="B156" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D156" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>47</v>
+      </c>
+      <c r="B157" t="s">
+        <v>8</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D157" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>47</v>
+      </c>
+      <c r="B158" t="s">
+        <v>9</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D158" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>52</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D159" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>52</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D160" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>52</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D161" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>52</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D162" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>